<commit_message>
Content viewer done. Few bugs to be fixed.
</commit_message>
<xml_diff>
--- a/Employee time sheet (weekly, monthly, yearly).xlsx
+++ b/Employee time sheet (weekly, monthly, yearly).xlsx
@@ -724,8 +724,8 @@
   </sheetPr>
   <dimension ref="B1:L141"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -772,7 +772,7 @@
       </c>
       <c r="J4" s="17">
         <f ca="1">SUMIF(B:B,"*Regular hours",C:D)</f>
-        <v>248</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
@@ -802,7 +802,7 @@
       </c>
       <c r="L5" s="17">
         <f ca="1">SUM(J4:J5)</f>
-        <v>248</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -1365,7 +1365,9 @@
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="E31" s="6">
+        <v>3</v>
+      </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -1380,7 +1382,9 @@
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="E32" s="6">
+        <v>3</v>
+      </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -1393,9 +1397,13 @@
       <c r="B33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="6"/>
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
       <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+      <c r="E33" s="6">
+        <v>2</v>
+      </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -1408,7 +1416,9 @@
       <c r="B34" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="6"/>
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -1423,7 +1433,9 @@
       <c r="B35" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="6"/>
+      <c r="C35" s="6">
+        <v>5</v>
+      </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -1438,7 +1450,9 @@
       <c r="B36" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="6"/>
+      <c r="C36" s="6">
+        <v>5</v>
+      </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
@@ -1470,7 +1484,7 @@
       </c>
       <c r="C38" s="10">
         <f t="shared" ref="C38:L38" si="2">SUM(C31:C37)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D38" s="10">
         <f t="shared" si="2"/>
@@ -1478,7 +1492,7 @@
       </c>
       <c r="E38" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F38" s="10">
         <f t="shared" si="2"/>
@@ -1516,7 +1530,7 @@
       </c>
       <c r="C39" s="12">
         <f>SUMIF(C30:L30,"&lt;&gt;Overtime",C38:L38)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D39" s="11" t="str">
         <f ca="1">TEXT(DATEVALUE(B30&amp;" 1, "&amp;YEAR(TODAY())),"mmm.")&amp;" total: Overtime"</f>

</xml_diff>